<commit_message>
Inserts with mistakes fixed
</commit_message>
<xml_diff>
--- a/Sprint 1/USBD04/Inserts/Dataset normalizado.xlsx
+++ b/Sprint 1/USBD04/Inserts/Dataset normalizado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Documentos\bddad2024\Sprint 1\USBD04\Inserts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F164E8-3D06-4D0A-A80D-473B97FB32CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321FB864-6F73-4129-9E02-9CBE090E612D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="700" activeTab="2" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="190">
   <si>
     <t>Name</t>
   </si>
@@ -613,10 +613,10 @@
     <t>Pan test and packaging</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>CustomerOrderId</t>
+  </si>
+  <si>
+    <t>ProductionDate</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2416,14 +2416,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE470C24-4865-4CED-BECB-9AD0BD718C1F}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G27" sqref="G27:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="6" width="14.5546875" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
@@ -2454,8 +2454,8 @@
       <c r="B2">
         <v>785</v>
       </c>
-      <c r="C2" t="s">
-        <v>137</v>
+      <c r="C2">
+        <v>2</v>
       </c>
       <c r="D2" s="1">
         <v>45550</v>
@@ -2466,7 +2466,7 @@
       <c r="F2" s="1"/>
       <c r="G2" t="str">
         <f>"INSERT INTO CustomerOrder(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; "," &amp; $C$1 &amp; "," &amp; $D$1 &amp; "," &amp; $E$1 &amp; ") VALUES(" &amp; A2 &amp; ", " &amp; B2 &amp; ", " &amp; C2 &amp; ", TO_DATE(" &amp; TEXT(D2,"'dd/MM/AAAA'") &amp; ", 'dd/MM/YYYY'), TO_DATE(" &amp; TEXT(E2,"'dd/MM/AAAA'") &amp; ", 'dd/MM/YYYY'));"</f>
-        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(1, 785, NULL, TO_DATE('15/09/2024', 'dd/MM/YYYY'), TO_DATE('23/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(1, 785, 2, TO_DATE('15/09/2024', 'dd/MM/YYYY'), TO_DATE('23/09/2024', 'dd/MM/YYYY'));</v>
       </c>
       <c r="S2" s="1"/>
     </row>
@@ -2477,8 +2477,8 @@
       <c r="B3">
         <v>657</v>
       </c>
-      <c r="C3" t="s">
-        <v>137</v>
+      <c r="C3">
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>45550</v>
@@ -2489,7 +2489,7 @@
       <c r="F3" s="1"/>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G8" si="0">"INSERT INTO CustomerOrder(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; "," &amp; $C$1 &amp; "," &amp; $D$1 &amp; "," &amp; $E$1 &amp; ") VALUES(" &amp; A3 &amp; ", " &amp; B3 &amp; ", " &amp; C3 &amp; ", TO_DATE(" &amp; TEXT(D3,"'dd/MM/AAAA'") &amp; ", 'dd/MM/YYYY'), TO_DATE(" &amp; TEXT(E3,"'dd/MM/AAAA'") &amp; ", 'dd/MM/YYYY'));"</f>
-        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(2, 657, NULL, TO_DATE('15/09/2024', 'dd/MM/YYYY'), TO_DATE('26/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(2, 657, 3, TO_DATE('15/09/2024', 'dd/MM/YYYY'), TO_DATE('26/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -2499,8 +2499,8 @@
       <c r="B4">
         <v>348</v>
       </c>
-      <c r="C4" t="s">
-        <v>137</v>
+      <c r="C4">
+        <v>4</v>
       </c>
       <c r="D4" s="1">
         <v>45550</v>
@@ -2511,7 +2511,7 @@
       <c r="F4" s="1"/>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(3, 348, NULL, TO_DATE('15/09/2024', 'dd/MM/YYYY'), TO_DATE('25/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(3, 348, 4, TO_DATE('15/09/2024', 'dd/MM/YYYY'), TO_DATE('25/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -2521,8 +2521,8 @@
       <c r="B5">
         <v>785</v>
       </c>
-      <c r="C5" t="s">
-        <v>137</v>
+      <c r="C5">
+        <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>45553</v>
@@ -2533,7 +2533,7 @@
       <c r="F5" s="1"/>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(4, 785, NULL, TO_DATE('18/09/2024', 'dd/MM/YYYY'), TO_DATE('25/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(4, 785, 2, TO_DATE('18/09/2024', 'dd/MM/YYYY'), TO_DATE('25/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -2543,8 +2543,8 @@
       <c r="B6">
         <v>657</v>
       </c>
-      <c r="C6" t="s">
-        <v>137</v>
+      <c r="C6">
+        <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>45553</v>
@@ -2555,7 +2555,7 @@
       <c r="F6" s="1"/>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(5, 657, NULL, TO_DATE('18/09/2024', 'dd/MM/YYYY'), TO_DATE('25/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(5, 657, 3, TO_DATE('18/09/2024', 'dd/MM/YYYY'), TO_DATE('25/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -2565,8 +2565,8 @@
       <c r="B7">
         <v>348</v>
       </c>
-      <c r="C7" t="s">
-        <v>137</v>
+      <c r="C7">
+        <v>4</v>
       </c>
       <c r="D7" s="1">
         <v>45553</v>
@@ -2577,7 +2577,7 @@
       <c r="F7" s="1"/>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(6, 348, NULL, TO_DATE('18/09/2024', 'dd/MM/YYYY'), TO_DATE('26/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(6, 348, 4, TO_DATE('18/09/2024', 'dd/MM/YYYY'), TO_DATE('26/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -2587,8 +2587,8 @@
       <c r="B8">
         <v>456</v>
       </c>
-      <c r="C8" t="s">
-        <v>137</v>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <v>45556</v>
@@ -2599,12 +2599,12 @@
       <c r="F8" s="1"/>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(7, 456, NULL, TO_DATE('21/09/2024', 'dd/MM/YYYY'), TO_DATE('26/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO CustomerOrder(Id,CustomerId,AddressId,DateOrder,DateDelivery) VALUES(7, 456, 1, TO_DATE('21/09/2024', 'dd/MM/YYYY'), TO_DATE('26/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s">
         <v>138</v>
@@ -2848,7 +2848,7 @@
         <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C26" t="s">
         <v>138</v>
@@ -2857,7 +2857,7 @@
         <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -2878,8 +2878,8 @@
         <v>45550</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>"INSERT INTO ProductionOrder(" &amp; $A$26 &amp; "," &amp; $B$26 &amp; "," &amp; $C$26 &amp; "," &amp; $D$26 &amp; "," &amp; $E$26 &amp; ") VALUES(" &amp; A27 &amp; "," &amp; B27 &amp; ", " &amp; C27 &amp; ", " &amp; D27 &amp; ", TO_DATE(" &amp; TEXT(E27,"'dd/MM/AAAA'") &amp; ", 'dd/MM/YYYY'));"</f>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(1,1, AS12945S22, 5, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
+        <f>"INSERT INTO ProductionOrder(" &amp; $A$26 &amp; "," &amp; $B$26 &amp; "," &amp; $C$26 &amp; "," &amp; $D$26 &amp; "," &amp; $E$26 &amp; ") VALUES(" &amp; A27 &amp; "," &amp; B27 &amp; ",'" &amp; C27 &amp; "', " &amp; D27 &amp; ", TO_DATE(" &amp; TEXT(E27,"'dd/MM/AAAA'") &amp; ", 'dd/MM/YYYY'));"</f>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(1,1,'AS12945S22', 5, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -2899,8 +2899,8 @@
         <v>45550</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f t="shared" ref="G28:G39" si="2">"INSERT INTO ProductionOrder(" &amp; $A$26 &amp; "," &amp; $B$26 &amp; "," &amp; $C$26 &amp; "," &amp; $D$26 &amp; "," &amp; $E$26 &amp; ") VALUES(" &amp; A28 &amp; "," &amp; B28 &amp; ", " &amp; C28 &amp; ", " &amp; D28 &amp; ", TO_DATE(" &amp; TEXT(E28,"'dd/MM/AAAA'") &amp; ", 'dd/MM/YYYY'));"</f>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(2,1, AS12945S20, 15, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
+        <f t="shared" ref="G28:G39" si="2">"INSERT INTO ProductionOrder(" &amp; $A$26 &amp; "," &amp; $B$26 &amp; "," &amp; $C$26 &amp; "," &amp; $D$26 &amp; "," &amp; $E$26 &amp; ") VALUES(" &amp; A28 &amp; "," &amp; B28 &amp; ",'" &amp; C28 &amp; "', " &amp; D28 &amp; ", TO_DATE(" &amp; TEXT(E28,"'dd/MM/AAAA'") &amp; ", 'dd/MM/YYYY'));"</f>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(2,1,'AS12945S20', 15, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="G29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(3,2, AS12945S22, 10, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(3,2,'AS12945S22', 10, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2942,7 +2942,7 @@
       </c>
       <c r="G30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(4,2, AS12945P17, 20, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(4,2,'AS12945P17', 20, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="G31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(5,3, AS12945S22, 10, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(5,3,'AS12945S22', 10, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -2984,7 +2984,7 @@
       </c>
       <c r="G32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(6,3, AS12945S20, 10, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(6,3,'AS12945S20', 10, TO_DATE('15/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -3005,7 +3005,7 @@
       </c>
       <c r="G33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(7,4, AS12945S20, 24, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(7,4,'AS12945S20', 24, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="G34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(8,4, AS12945S22, 16, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(8,4,'AS12945S22', 16, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="G35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(9,4, AS12945S17, 8, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(9,4,'AS12945S17', 8, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="G36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(10,5, AS12945S22, 12, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(10,5,'AS12945S22', 12, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -3089,7 +3089,7 @@
       </c>
       <c r="G37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(11,6, AS12945S17, 8, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(11,6,'AS12945S17', 8, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="G38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(12,6, AS12945P17, 16, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(12,6,'AS12945P17', 16, TO_DATE('18/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="G39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,Date) VALUES(13,7, AS12945S22, 8, TO_DATE('21/09/2024', 'dd/MM/YYYY'));</v>
+        <v>INSERT INTO ProductionOrder(Id,CustomerOrderId,ProductId,Quantity,ProductionDate) VALUES(13,7,'AS12945S22', 8, TO_DATE('21/09/2024', 'dd/MM/YYYY'));</v>
       </c>
     </row>
   </sheetData>
@@ -4936,6 +4936,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005CAEFE7FC9D8B84EBE55524C48F58D03" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="497854f89e4a3d7bf883e8e815c91d37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0" xmlns:ns4="c83fef03-7e53-47dc-8a06-28f89aa017e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19b7ffbcacb703e844d38f10494d74a9" ns3:_="" ns4:_="">
     <xsd:import namespace="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0"/>
@@ -5168,24 +5185,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7026BE-4F45-4595-B98C-E9D8129D4591}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c83fef03-7e53-47dc-8a06-28f89aa017e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C8F835-22B2-4A5C-B33C-2EBD4DAC13D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21BE2CCF-9747-4435-B7C5-28A62B986CF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5202,29 +5227,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C8F835-22B2-4A5C-B33C-2EBD4DAC13D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7026BE-4F45-4595-B98C-E9D8129D4591}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c83fef03-7e53-47dc-8a06-28f89aa017e1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>